<commit_message>
Modifications to *.aim files - to allow ESP-r to calculate the ELA based on the calculated volume of each house.
Updates to Optimization command and ini files for generic model.
</commit_message>
<xml_diff>
--- a/OptFramework/GenericHome-base/GenericModel Window size calculation.xlsx
+++ b/OptFramework/GenericHome-base/GenericModel Window size calculation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="79">
   <si>
     <t>window geometry calculations</t>
   </si>
@@ -162,9 +162,6 @@
     <t xml:space="preserve">1,4,3,2 </t>
   </si>
   <si>
-    <t>surface</t>
-  </si>
-  <si>
     <t>wall-1</t>
   </si>
   <si>
@@ -247,6 +244,15 @@
   </si>
   <si>
     <t>&lt;win-wall-4-left&gt;</t>
+  </si>
+  <si>
+    <t>Surface</t>
+  </si>
+  <si>
+    <t>&lt;Opt-Eave-Height&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Opt-Bsm-Depth&gt;</t>
   </si>
 </sst>
 </file>
@@ -254,9 +260,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +310,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -325,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -355,22 +369,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,18 +687,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -697,11 +712,11 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="13" t="s">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="G1" s="13"/>
       <c r="H1" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -711,21 +726,21 @@
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
-        <v>123</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="13">
+        <v>206</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G2" t="s">
         <v>42</v>
       </c>
       <c r="H2">
-        <f>+(B21-B20)*(D26-D21)</f>
-        <v>31.774999999999995</v>
+        <f>+(B23-B22)*(D28-D23)</f>
+        <v>46.172413793103452</v>
       </c>
       <c r="I2" t="s">
         <v>4</v>
@@ -739,20 +754,20 @@
         <v>13</v>
       </c>
       <c r="C3" s="1">
-        <v>12</v>
+        <v>14.5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G3" t="s">
         <v>43</v>
       </c>
       <c r="H3">
-        <f>+(C22-C21)*(D26-D22)</f>
-        <v>37.199999999999996</v>
+        <f>+(C24-C23)*(D28-D24)</f>
+        <v>47.125</v>
       </c>
       <c r="I3" t="s">
         <v>4</v>
@@ -767,20 +782,20 @@
       </c>
       <c r="C4" s="2">
         <f>+C2/C3</f>
-        <v>10.25</v>
+        <v>14.206896551724139</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
       </c>
       <c r="H4">
-        <f>+(B22-B23)*(D26-D23)</f>
-        <v>31.774999999999995</v>
+        <f>+(B24-B25)*(D28-D25)</f>
+        <v>46.172413793103452</v>
       </c>
       <c r="I4" t="s">
         <v>4</v>
@@ -791,21 +806,21 @@
         <v>2</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="1">
+      <c r="C5" s="13">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="13" t="s">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
       </c>
       <c r="H5">
-        <f>+(C23-C20)*(D27-D23)</f>
-        <v>37.199999999999996</v>
+        <f>+(C25-C22)*(D29-D25)</f>
+        <v>47.125</v>
       </c>
       <c r="I5" t="s">
         <v>4</v>
@@ -818,296 +833,288 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="13">
         <v>2.5</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
         <v>46</v>
       </c>
       <c r="H6">
-        <f>+(B25*C26)</f>
-        <v>123</v>
+        <f>+(B27*C28)</f>
+        <v>206</v>
       </c>
       <c r="I6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5.6</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="13">
+        <v>2</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
       </c>
       <c r="H7">
-        <f>+C23*B22</f>
-        <v>123</v>
+        <f>+C25*B24</f>
+        <v>206</v>
       </c>
       <c r="I7" t="s">
         <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C8" s="8">
-        <f>+$D$29</f>
-        <v>3</v>
-      </c>
-      <c r="D8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5.75</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="15">
         <f>+H2*$C$5/100</f>
-        <v>4.7662499999999994</v>
+        <v>6.9258620689655173</v>
       </c>
       <c r="I8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="J8" s="19">
         <f>+H8/K8</f>
-        <v>3.0750000000000002</v>
+        <v>4.2620689655172415</v>
       </c>
       <c r="K8" s="9">
-        <f>+($C$7-$C$6)/2</f>
-        <v>1.5499999999999998</v>
+        <f>+($C$8-$C$6)/2</f>
+        <v>1.625</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="8">
-        <f>+$D$31</f>
-        <v>4.55</v>
-      </c>
-      <c r="D9" s="1"/>
+      <c r="B9" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="23">
+        <f>+C8-C7</f>
+        <v>3.75</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H9" s="16">
-        <f t="shared" ref="H9:H11" si="0">+H3*$C$5/100</f>
-        <v>5.5799999999999992</v>
+        <f>+H3*$C$5/100</f>
+        <v>7.0687499999999996</v>
       </c>
       <c r="I9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="J9" s="20">
-        <f t="shared" ref="J9:J11" si="1">+H9/K9</f>
-        <v>3.6</v>
+        <f t="shared" ref="J9:J11" si="0">+H9/K9</f>
+        <v>4.3499999999999996</v>
       </c>
       <c r="K9" s="11">
-        <f t="shared" ref="K9:K11" si="2">+($C$7-$C$6)/2</f>
-        <v>1.5499999999999998</v>
+        <f t="shared" ref="K9:K11" si="1">+($C$8-$C$6)/2</f>
+        <v>1.625</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C10" s="8">
-        <f>+$B$28</f>
-        <v>0.5</v>
-      </c>
+        <f>+$D$31</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="F10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="17">
-        <f t="shared" si="0"/>
-        <v>4.7662499999999994</v>
+        <f>+H4*$C$5/100</f>
+        <v>6.9258620689655173</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="21">
+        <f t="shared" si="0"/>
+        <v>4.2620689655172415</v>
+      </c>
+      <c r="K10" s="7">
         <f t="shared" si="1"/>
-        <v>3.0750000000000002</v>
-      </c>
-      <c r="K10" s="7">
-        <f t="shared" si="2"/>
-        <v>1.5499999999999998</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="15">
-        <f>+$B$29</f>
-        <v>3.5750000000000002</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C11" s="8">
+        <f>+$D$33</f>
+        <v>4.625</v>
+      </c>
+      <c r="D11" s="1"/>
       <c r="F11" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H11" s="18">
-        <f t="shared" si="0"/>
-        <v>5.5799999999999992</v>
+        <f>+H5*$C$5/100</f>
+        <v>7.0687499999999996</v>
       </c>
       <c r="I11" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J11" s="22">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="K11" s="14">
         <f t="shared" si="1"/>
-        <v>3.6</v>
-      </c>
-      <c r="K11" s="14">
-        <f t="shared" si="2"/>
-        <v>1.5499999999999998</v>
+        <v>1.625</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="8">
+        <f>+$B$30</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="15">
+        <f>+$B$31</f>
+        <v>4.7620689655172415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="10">
+        <f>+$C$34</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C12" s="10">
-        <f>+$C$32</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="16">
-        <f>+$C$33</f>
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
+      <c r="C15" s="16">
+        <f>+$C$35</f>
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="17">
+        <f>+$B$38</f>
+        <v>13.706896551724139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C14" s="17">
-        <f>+$B$36</f>
-        <v>9.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
+      <c r="C17" s="17">
+        <f>+$B$39</f>
+        <v>9.4448275862068982</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C15" s="17">
-        <f>+$B$37</f>
-        <v>6.6749999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+      <c r="C18" s="12">
+        <f>+$C$42</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="12">
-        <f>+$C$40</f>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="18">
-        <f>+$C$41</f>
-        <v>7.9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="18">
+        <f>+$C$43</f>
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="3">
-        <v>0</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0</v>
-      </c>
-      <c r="D20" s="3">
-        <f>+$C$6</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4">
-        <f>+$C$4</f>
-        <v>10.25</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0</v>
-      </c>
-      <c r="D21" s="3">
-        <f>+$C$6</f>
-        <v>2.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4">
-        <f>+$C$4</f>
-        <v>10.25</v>
+        <v>15</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0</v>
       </c>
       <c r="C22" s="3">
-        <f>+$C$3</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D22" s="3">
         <f>+$C$6</f>
@@ -1116,14 +1123,14 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="3">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="B23" s="4">
+        <f>+$C$4</f>
+        <v>14.206896551724139</v>
       </c>
       <c r="C23" s="3">
-        <f>+$C$3</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D23" s="3">
         <f>+$C$6</f>
@@ -1132,338 +1139,371 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="3">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="B24" s="4">
+        <f>+$C$4</f>
+        <v>14.206896551724139</v>
       </c>
       <c r="C24" s="3">
-        <v>0</v>
+        <f>+$C$3</f>
+        <v>14.5</v>
       </c>
       <c r="D24" s="3">
-        <f>+$C$7</f>
-        <v>5.6</v>
+        <f>+$C$6</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4">
-        <f t="shared" ref="B25:B26" si="3">+$C$4</f>
-        <v>10.25</v>
+        <v>18</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
       </c>
       <c r="C25" s="3">
-        <v>0</v>
+        <f>+$C$3</f>
+        <v>14.5</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" ref="D25:D27" si="4">+$C$7</f>
-        <v>5.6</v>
+        <f>+$C$6</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4">
-        <f t="shared" si="3"/>
-        <v>10.25</v>
+        <v>19</v>
+      </c>
+      <c r="B26" s="3">
+        <v>0</v>
       </c>
       <c r="C26" s="3">
-        <f>+$C$3</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="4"/>
-        <v>5.6</v>
+        <f>+$C$8</f>
+        <v>5.75</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4">
+        <f t="shared" ref="B27:B28" si="2">+$C$4</f>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C27" s="3">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" ref="D27:D29" si="3">+$C$8</f>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4">
+        <f t="shared" si="2"/>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C28" s="3">
+        <f>+$C$3</f>
+        <v>14.5</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
         <f>+$C$3</f>
-        <v>12</v>
-      </c>
-      <c r="D27" s="3">
-        <f t="shared" si="4"/>
-        <v>5.6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="9">
-        <f>+B20+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="C28" s="9">
-        <f>+C20</f>
-        <v>0</v>
-      </c>
-      <c r="D28" s="9">
-        <f>+$D$20+0.5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="19">
-        <f>+B28+$J$8</f>
-        <v>3.5750000000000002</v>
-      </c>
-      <c r="C29" s="9">
-        <f>+C21</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="9">
-        <f>+$D$20+0.5</f>
-        <v>3</v>
+        <v>14.5</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="3"/>
+        <v>5.75</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="19">
-        <f>+B28+$J$8</f>
-        <v>3.5750000000000002</v>
+        <v>23</v>
+      </c>
+      <c r="B30" s="9">
+        <f>+B22+0.5</f>
+        <v>0.5</v>
       </c>
       <c r="C30" s="9">
-        <f>+C24</f>
+        <f>+C22</f>
         <v>0</v>
       </c>
       <c r="D30" s="9">
-        <f>+D28+$K$8</f>
-        <v>4.55</v>
+        <f>+$D$22+0.5</f>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="19">
+        <f>+B30+$J$8</f>
+        <v>4.7620689655172415</v>
+      </c>
+      <c r="C31" s="9">
+        <f>+C23</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <f>+$D$22+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="19">
+        <f>+B30+$J$8</f>
+        <v>4.7620689655172415</v>
+      </c>
+      <c r="C32" s="9">
+        <f>+C26</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <f>+D30+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="9">
+      <c r="B33" s="9">
+        <f>+B30</f>
+        <v>0.5</v>
+      </c>
+      <c r="C33" s="9">
+        <f>+C27</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <f>+D31+$K$8</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="20">
+        <f>+B23</f>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C34" s="11">
+        <f>+C23+0.5</f>
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="11">
+        <f>+D23+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="20">
+        <f>+B24</f>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C35" s="11">
+        <f>+C34+J9</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D35" s="11">
+        <f>+D24+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="20">
         <f>+B28</f>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C36" s="11">
+        <f>+C34+$J$9</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="D36" s="11">
+        <f>+D34+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="20">
+        <f>+B27</f>
+        <v>14.206896551724139</v>
+      </c>
+      <c r="C37" s="11">
+        <f>+C27+0.5</f>
         <v>0.5</v>
       </c>
-      <c r="C31" s="9">
+      <c r="D37" s="11">
+        <f>+D35+$K$9</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="21">
+        <f>+B24-0.5</f>
+        <v>13.706896551724139</v>
+      </c>
+      <c r="C38" s="7">
+        <f>+C24</f>
+        <v>14.5</v>
+      </c>
+      <c r="D38" s="7">
+        <f>+D24+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="21">
+        <f>+B38-$J$10</f>
+        <v>9.4448275862068982</v>
+      </c>
+      <c r="C39" s="7">
         <f>+C25</f>
-        <v>0</v>
-      </c>
-      <c r="D31" s="9">
-        <f>+D29+$K$8</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="20">
-        <f>+B21</f>
-        <v>10.25</v>
-      </c>
-      <c r="C32" s="11">
-        <f>+C21+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="D32" s="11">
-        <f>+D21+0.5</f>
+        <v>14.5</v>
+      </c>
+      <c r="D39" s="7">
+        <f>+D25+0.5</f>
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="20">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="21">
+        <f>+B39</f>
+        <v>9.4448275862068982</v>
+      </c>
+      <c r="C40" s="7">
+        <f>+C39</f>
+        <v>14.5</v>
+      </c>
+      <c r="D40" s="7">
+        <f>+D39+$K$10</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="21">
+        <f>+B38</f>
+        <v>13.706896551724139</v>
+      </c>
+      <c r="C41" s="7">
+        <f>+C40</f>
+        <v>14.5</v>
+      </c>
+      <c r="D41" s="7">
+        <f>+D40</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="14">
+        <f>+B25</f>
+        <v>0</v>
+      </c>
+      <c r="C42" s="14">
+        <f>+C25-0.5</f>
+        <v>14</v>
+      </c>
+      <c r="D42" s="14">
+        <f>+D25+0.5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="14">
         <f>+B22</f>
-        <v>10.25</v>
-      </c>
-      <c r="C33" s="11">
-        <f>+C32+J9</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C43" s="14">
+        <f>+C42-$J$11</f>
+        <v>9.65</v>
+      </c>
+      <c r="D43" s="14">
         <f>+D22+0.5</f>
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" s="20">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="14">
         <f>+B26</f>
-        <v>10.25</v>
-      </c>
-      <c r="C34" s="11">
-        <f>+C32+$J$9</f>
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="D34" s="11">
-        <f>+D32+$K$9</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="20">
-        <f>+B25</f>
-        <v>10.25</v>
-      </c>
-      <c r="C35" s="11">
-        <f>+C25+0.5</f>
-        <v>0.5</v>
-      </c>
-      <c r="D35" s="11">
-        <f>+D33+$K$9</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B36" s="21">
-        <f>+B22-0.5</f>
-        <v>9.75</v>
-      </c>
-      <c r="C36" s="7">
-        <f>+C22</f>
-        <v>12</v>
-      </c>
-      <c r="D36" s="7">
-        <f>+D22+0.5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B37" s="21">
-        <f>+B36-$J$10</f>
-        <v>6.6749999999999998</v>
-      </c>
-      <c r="C37" s="7">
-        <f>+C23</f>
-        <v>12</v>
-      </c>
-      <c r="D37" s="7">
-        <f>+D23+0.5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="21">
-        <f>+B37</f>
-        <v>6.6749999999999998</v>
-      </c>
-      <c r="C38" s="7">
-        <f>+C37</f>
-        <v>12</v>
-      </c>
-      <c r="D38" s="7">
-        <f>+D37+$K$10</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="21">
-        <f>+B36</f>
-        <v>9.75</v>
-      </c>
-      <c r="C39" s="7">
-        <f>+C38</f>
-        <v>12</v>
-      </c>
-      <c r="D39" s="7">
-        <f>+D38</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="14">
-        <f>+B23</f>
-        <v>0</v>
-      </c>
-      <c r="C40" s="14">
-        <f>+C23-0.5</f>
-        <v>11.5</v>
-      </c>
-      <c r="D40" s="14">
-        <f>+D23+0.5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="14">
-        <f>+B20</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="14">
-        <f>+C40-$J$11</f>
-        <v>7.9</v>
-      </c>
-      <c r="D41" s="14">
-        <f>+D20+0.5</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B42" s="14">
-        <f>+B24</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="14">
-        <f>+C41</f>
-        <v>7.9</v>
-      </c>
-      <c r="D42" s="14">
-        <f>+D41+$K$11</f>
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="14">
+        <f>+C43</f>
+        <v>9.65</v>
+      </c>
+      <c r="D44" s="14">
+        <f>+D43+$K$11</f>
+        <v>4.625</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="14">
-        <f>+B27</f>
-        <v>0</v>
-      </c>
-      <c r="C43" s="14">
-        <f>+C40</f>
-        <v>11.5</v>
-      </c>
-      <c r="D43" s="14">
-        <f>+D42</f>
-        <v>4.55</v>
+      <c r="B45" s="14">
+        <f>+B29</f>
+        <v>0</v>
+      </c>
+      <c r="C45" s="14">
+        <f>+C42</f>
+        <v>14</v>
+      </c>
+      <c r="D45" s="14">
+        <f>+D44</f>
+        <v>4.625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>